<commit_message>
Update 12-22-18 ~ ERD Virtualization
</commit_message>
<xml_diff>
--- a/GegevensTabels.xlsx
+++ b/GegevensTabels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Documents\School\Avans\P2\RDB + Pro2 Eindopdracht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Egberts\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28F220D-991B-4233-95F1-026B4DA85094}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDFD8C4-CDE2-4A01-907E-8B78B170930C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{125B87A5-2ABC-419A-83C9-B8206006D560}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7275" xr2:uid="{125B87A5-2ABC-419A-83C9-B8206006D560}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Abonnee</t>
   </si>
@@ -57,21 +57,12 @@
     <t>Profiel</t>
   </si>
   <si>
-    <t>Adres</t>
-  </si>
-  <si>
-    <t>Voorkeur</t>
-  </si>
-  <si>
     <t>Kijkgedrag</t>
   </si>
   <si>
     <t>Leeftijd</t>
   </si>
   <si>
-    <t>Progrm.</t>
-  </si>
-  <si>
     <t>Prfl. Naam</t>
   </si>
   <si>
@@ -103,13 +94,22 @@
   </si>
   <si>
     <t>Serie</t>
+  </si>
+  <si>
+    <t>TijdsDuur minuten</t>
+  </si>
+  <si>
+    <t>AbonneeID</t>
+  </si>
+  <si>
+    <t>Profiel Naam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +119,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,10 +154,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -464,21 +473,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CAEE71-AFF1-45DA-A7C9-638BDC58C608}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -496,88 +511,101 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>